<commit_message>
message for opposite peaks
</commit_message>
<xml_diff>
--- a/data/Resultats exp bag_couverts/Resultats exp bag_couverts/Tableau récapitulatif - new algo.xlsx
+++ b/data/Resultats exp bag_couverts/Resultats exp bag_couverts/Tableau récapitulatif - new algo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abarb\Documents\travail\stage et4\travail\codePlateau\Resultats exp bag_couverts\Resultats exp bag_couverts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abarb\Documents\travail\stage et4\travail\codePlateau\data\Resultats exp bag_couverts\Resultats exp bag_couverts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032D5D1F-CF54-4F02-AF5E-8235A791422A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB436CEE-C3B1-4E30-8B4F-7898ACAA23E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2467,31 +2467,31 @@
         <v>1</v>
       </c>
       <c r="K3" s="6">
-        <v>148.21100000000001</v>
+        <v>169.84199999999998</v>
       </c>
       <c r="L3" s="6">
-        <v>169</v>
+        <v>208</v>
       </c>
       <c r="M3" s="6">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="N3" s="6">
-        <v>-178.32000000000005</v>
+        <v>60.252999999999929</v>
       </c>
       <c r="O3" s="6">
-        <v>-17.832000000000001</v>
+        <v>5.4779999999999998</v>
       </c>
       <c r="P3" s="6">
         <v>7.0779999999999745</v>
       </c>
       <c r="Q3" s="6">
-        <v>-235.13600000000008</v>
+        <v>0.20100000000002183</v>
       </c>
       <c r="R3" s="6">
-        <v>-120.3</v>
+        <v>35.5</v>
       </c>
       <c r="S3" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T3" s="6" t="s">
         <v>37</v>
@@ -2579,13 +2579,13 @@
         <v>2</v>
       </c>
       <c r="K5" s="6">
-        <v>257.44900000000001</v>
+        <v>272.40999999999997</v>
       </c>
       <c r="L5" s="6">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="M5" s="6">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N5" s="6">
         <v>92.68900000000005</v>
@@ -2600,7 +2600,7 @@
         <v>0.20199999999999818</v>
       </c>
       <c r="R5" s="6">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S5" s="6">
         <v>18</v>
@@ -2644,31 +2644,31 @@
         <v>2</v>
       </c>
       <c r="K6" s="6">
-        <v>219.97500000000002</v>
+        <v>226.44399999999996</v>
       </c>
       <c r="L6" s="6">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="M6" s="6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N6" s="6">
-        <v>-146.97999999999979</v>
+        <v>90.380000000000223</v>
       </c>
       <c r="O6" s="6">
-        <v>-9.1859999999999999</v>
+        <v>5.3159999999999998</v>
       </c>
       <c r="P6" s="6">
         <v>8.4920000000000755</v>
       </c>
       <c r="Q6" s="6">
-        <v>-233.31700000000001</v>
+        <v>0.20299999999997453</v>
       </c>
       <c r="R6" s="6">
-        <v>-66.8</v>
+        <v>39.9</v>
       </c>
       <c r="S6" s="6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="T6" s="6" t="s">
         <v>39</v>
@@ -2709,13 +2709,13 @@
         <v>2</v>
       </c>
       <c r="K7" s="6">
-        <v>462.07200000000012</v>
+        <v>495.83199999999999</v>
       </c>
       <c r="L7" s="6">
         <v>177</v>
       </c>
       <c r="M7" s="6">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="N7" s="6">
         <v>116.44800000000055</v>
@@ -2730,7 +2730,7 @@
         <v>0.20100000000002183</v>
       </c>
       <c r="R7" s="6">
-        <v>25.2</v>
+        <v>23.5</v>
       </c>
       <c r="S7" s="6">
         <v>19</v>
@@ -2774,13 +2774,13 @@
         <v>1</v>
       </c>
       <c r="K8" s="6">
-        <v>279.14300000000003</v>
+        <v>288.45399999999995</v>
       </c>
       <c r="L8" s="6">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="M8" s="6">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N8" s="6">
         <v>87.703999999999922</v>
@@ -2795,7 +2795,7 @@
         <v>0.21600000000000819</v>
       </c>
       <c r="R8" s="6">
-        <v>31.4</v>
+        <v>30.4</v>
       </c>
       <c r="S8" s="6">
         <v>20</v>
@@ -2839,13 +2839,13 @@
         <v>1</v>
       </c>
       <c r="K9" s="6">
-        <v>221.21199999999999</v>
+        <v>226.40899999999999</v>
       </c>
       <c r="L9" s="6">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M9" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N9" s="6">
         <v>53.925999999999704</v>
@@ -2860,7 +2860,7 @@
         <v>0.21600000000000819</v>
       </c>
       <c r="R9" s="6">
-        <v>24.4</v>
+        <v>23.8</v>
       </c>
       <c r="S9" s="6">
         <v>20</v>
@@ -2904,13 +2904,13 @@
         <v>1</v>
       </c>
       <c r="K10" s="6">
-        <v>51.322000000000003</v>
+        <v>61.499000000000024</v>
       </c>
       <c r="L10" s="6">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="M10" s="6">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="N10" s="6">
         <v>32.2650000000001</v>
@@ -2925,7 +2925,7 @@
         <v>0.43299999999999272</v>
       </c>
       <c r="R10" s="6">
-        <v>62.9</v>
+        <v>52.5</v>
       </c>
       <c r="S10" s="6">
         <v>5</v>
@@ -2969,13 +2969,13 @@
         <v>2</v>
       </c>
       <c r="K11" s="6">
-        <v>216.55700000000002</v>
+        <v>280.44200000000001</v>
       </c>
       <c r="L11" s="6">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="M11" s="6">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="N11" s="6">
         <v>108.49500000000009</v>
@@ -2990,7 +2990,7 @@
         <v>0.21600000000000819</v>
       </c>
       <c r="R11" s="6">
-        <v>50.1</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="S11" s="6">
         <v>15</v>
@@ -3034,13 +3034,13 @@
         <v>2</v>
       </c>
       <c r="K12" s="6">
-        <v>211.90000000000009</v>
+        <v>219.04600000000005</v>
       </c>
       <c r="L12" s="6">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="M12" s="6">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N12" s="6">
         <v>83.271000000000299</v>
@@ -3055,7 +3055,7 @@
         <v>0.64999999999997726</v>
       </c>
       <c r="R12" s="6">
-        <v>39.299999999999997</v>
+        <v>38</v>
       </c>
       <c r="S12" s="6">
         <v>16</v>
@@ -3099,13 +3099,13 @@
         <v>2</v>
       </c>
       <c r="K13" s="6">
-        <v>379.29600000000005</v>
+        <v>446.64699999999993</v>
       </c>
       <c r="L13" s="6">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M13" s="6">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="N13" s="6">
         <v>197.93200000000093</v>
@@ -3120,7 +3120,7 @@
         <v>0.43299999999999272</v>
       </c>
       <c r="R13" s="6">
-        <v>52.2</v>
+        <v>44.3</v>
       </c>
       <c r="S13" s="6">
         <v>14</v>
@@ -3359,13 +3359,13 @@
         <v>4</v>
       </c>
       <c r="K17" s="6">
-        <v>272.43</v>
+        <v>291.48700000000002</v>
       </c>
       <c r="L17" s="6">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="M17" s="6">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N17" s="6">
         <v>91.391999999999882</v>
@@ -3380,7 +3380,7 @@
         <v>0.21699999999998454</v>
       </c>
       <c r="R17" s="6">
-        <v>33.5</v>
+        <v>31.4</v>
       </c>
       <c r="S17" s="6">
         <v>14</v>
@@ -3424,13 +3424,13 @@
         <v>4</v>
       </c>
       <c r="K18" s="6">
-        <v>234.20500000000004</v>
+        <v>236.37</v>
       </c>
       <c r="L18" s="6">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="M18" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N18" s="6">
         <v>84.456000000000017</v>
@@ -3445,7 +3445,7 @@
         <v>0.21699999999998454</v>
       </c>
       <c r="R18" s="6">
-        <v>36.1</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="S18" s="6">
         <v>11</v>
@@ -3489,13 +3489,13 @@
         <v>4</v>
       </c>
       <c r="K19" s="6">
-        <v>423.47500000000002</v>
+        <v>429.322</v>
       </c>
       <c r="L19" s="6">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="M19" s="6">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N19" s="6">
         <v>149.7529999999997</v>
@@ -3510,7 +3510,7 @@
         <v>0.64900000000000091</v>
       </c>
       <c r="R19" s="6">
-        <v>35.4</v>
+        <v>34.9</v>
       </c>
       <c r="S19" s="6">
         <v>22</v>
@@ -3554,13 +3554,13 @@
         <v>1</v>
       </c>
       <c r="K20" s="6">
-        <v>229.05300000000005</v>
+        <v>230.46899999999999</v>
       </c>
       <c r="L20" s="6">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="M20" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N20" s="6">
         <v>127.27499999999986</v>
@@ -3575,7 +3575,7 @@
         <v>0.20199999999999818</v>
       </c>
       <c r="R20" s="6">
-        <v>55.6</v>
+        <v>55.2</v>
       </c>
       <c r="S20" s="6">
         <v>16</v>
@@ -3619,13 +3619,13 @@
         <v>1</v>
       </c>
       <c r="K21" s="6">
-        <v>227.19399999999996</v>
+        <v>234.67899999999997</v>
       </c>
       <c r="L21" s="6">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="M21" s="6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N21" s="6">
         <v>123.40800000000013</v>
@@ -3640,7 +3640,7 @@
         <v>0.40399999999999636</v>
       </c>
       <c r="R21" s="6">
-        <v>54.3</v>
+        <v>52.6</v>
       </c>
       <c r="S21" s="6">
         <v>12</v>
@@ -3749,13 +3749,13 @@
         <v>2</v>
       </c>
       <c r="K23" s="6">
-        <v>226.22100000000006</v>
+        <v>231.47999999999996</v>
       </c>
       <c r="L23" s="6">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M23" s="6">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N23" s="6">
         <v>116.14200000000011</v>
@@ -3770,7 +3770,7 @@
         <v>0.6069999999999709</v>
       </c>
       <c r="R23" s="6">
-        <v>51.3</v>
+        <v>50.2</v>
       </c>
       <c r="S23" s="6">
         <v>19</v>
@@ -3879,13 +3879,13 @@
         <v>2</v>
       </c>
       <c r="K25" s="6">
-        <v>149.29700000000003</v>
+        <v>198.25299999999993</v>
       </c>
       <c r="L25" s="6">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="M25" s="6">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="N25" s="6">
         <v>103.78000000000031</v>
@@ -3900,7 +3900,7 @@
         <v>0.20300000000020191</v>
       </c>
       <c r="R25" s="6">
-        <v>69.5</v>
+        <v>52.3</v>
       </c>
       <c r="S25" s="6">
         <v>12</v>
@@ -3944,13 +3944,13 @@
         <v>1</v>
       </c>
       <c r="K26" s="6">
-        <v>199.298</v>
+        <v>201.68100000000004</v>
       </c>
       <c r="L26" s="6">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M26" s="6">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N26" s="6">
         <v>71.051000000000045</v>
@@ -3965,7 +3965,7 @@
         <v>0.43299999999999272</v>
       </c>
       <c r="R26" s="6">
-        <v>35.700000000000003</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="S26" s="6">
         <v>18</v>
@@ -4074,13 +4074,13 @@
         <v>1</v>
       </c>
       <c r="K28" s="6">
-        <v>253.88599999999997</v>
+        <v>260.60100000000011</v>
       </c>
       <c r="L28" s="6">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="M28" s="6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N28" s="6">
         <v>62.845000000000482</v>
@@ -4095,7 +4095,7 @@
         <v>0.2159999999998945</v>
       </c>
       <c r="R28" s="6">
-        <v>24.8</v>
+        <v>24.1</v>
       </c>
       <c r="S28" s="6">
         <v>12</v>
@@ -4139,13 +4139,13 @@
         <v>2</v>
       </c>
       <c r="K29" s="6">
-        <v>216.19400000000002</v>
+        <v>222.04399999999998</v>
       </c>
       <c r="L29" s="6">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M29" s="6">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N29" s="6">
         <v>89.544000000000267</v>
@@ -4160,7 +4160,7 @@
         <v>0.21699999999998454</v>
       </c>
       <c r="R29" s="6">
-        <v>41.4</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="S29" s="6">
         <v>23</v>
@@ -4204,13 +4204,13 @@
         <v>2</v>
       </c>
       <c r="K30" s="6">
-        <v>170.48699999999997</v>
+        <v>230.92499999999995</v>
       </c>
       <c r="L30" s="6">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="M30" s="6">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="N30" s="6">
         <v>55.888000000000034</v>
@@ -4225,7 +4225,7 @@
         <v>0.21600000000000819</v>
       </c>
       <c r="R30" s="6">
-        <v>32.799999999999997</v>
+        <v>24.2</v>
       </c>
       <c r="S30" s="6">
         <v>12</v>
@@ -4334,13 +4334,13 @@
         <v>3</v>
       </c>
       <c r="K32" s="6">
-        <v>1073.5820000000001</v>
+        <v>1092.6420000000001</v>
       </c>
       <c r="L32" s="6">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="M32" s="6">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="N32" s="6">
         <v>413.84799999999973</v>
@@ -4355,7 +4355,7 @@
         <v>0.21600000000000819</v>
       </c>
       <c r="R32" s="6">
-        <v>38.5</v>
+        <v>37.9</v>
       </c>
       <c r="S32" s="6">
         <v>50</v>

</xml_diff>